<commit_message>
Se agrega avance de goldbach_openmp_mpi
</commit_message>
<xml_diff>
--- a/report/perfMeasure.xlsx
+++ b/report/perfMeasure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\estebancb03\Documents\Concurrente22a_Esteban_Castaneda\tareas\goldbach_optimization\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\estebancb03\Documents\Concurrente22a_Esteban_Castaneda\tareas\goldbach_openmp_mpi\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D420A1-0569-4058-8B0E-828AA85D2DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36788D3B-BBCC-455F-BD9D-38B5144B5A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -227,6 +227,48 @@
         </r>
       </text>
     </comment>
+    <comment ref="O2" authorId="1" shapeId="0" xr:uid="{3C810B61-73A6-4A15-B5F4-C8788135A95A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Liberation Sans1"/>
+          </rPr>
+          <t>Tantos hilos como números recibe el programa en la entrada estándar</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Liberation Sans1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P2" authorId="1" shapeId="0" xr:uid="{7ABC4AD2-3A34-49FE-9B1F-3F50BF79A806}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Liberation Sans1"/>
+          </rPr>
+          <t>Tantos hilos como números recibe el programa en la entrada estándar</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Liberation Sans1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
@@ -292,7 +334,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t>CPU C=</t>
   </si>
@@ -400,6 +442,18 @@
   </si>
   <si>
     <t>Optimización3</t>
+  </si>
+  <si>
+    <t>OpenMP</t>
+  </si>
+  <si>
+    <t>OpenMP-MPI</t>
+  </si>
+  <si>
+    <t>MPI</t>
+  </si>
+  <si>
+    <t>Create a graph for comparing serial and OpenMP version using two vertical axes here</t>
   </si>
 </sst>
 </file>
@@ -558,7 +612,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -663,6 +717,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -692,7 +770,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -739,9 +817,6 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -749,6 +824,28 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Accent" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2437,6 +2534,436 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Comparación</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> #3: Tarea #2 vs OpenMP</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tareas!$E$67</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Incremento de velocidad (veces)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tareas!$C$68:$C$69</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Tarea2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OpenMP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tareas!$E$68:$E$69</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>190.87</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7E8D-44A8-B741-5478AE91BA60}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tareas!$F$67</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Eficiencia (veces)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tareas!$C$68:$C$69</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Tarea2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OpenMP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tareas!$F$68:$F$69</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.91</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7E8D-44A8-B741-5478AE91BA60}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1760286464"/>
+        <c:axId val="1760286880"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1760286464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1760286880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1760286880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1760286464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
@@ -2548,6 +3075,43 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="322">
   <cs:axisTitle>
@@ -3568,6 +4132,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4750,6 +5817,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>14286</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>581024</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Gráfico 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46A07A8C-5C97-4745-F311-A3B4AA66CABB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5050,10 +6153,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O60"/>
+  <dimension ref="A1:T69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="P73" sqref="P73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5063,10 +6166,12 @@
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="7" width="8.5546875" customWidth="1"/>
     <col min="8" max="8" width="8.21875" customWidth="1"/>
-    <col min="9" max="1023" width="7.33203125" customWidth="1"/>
+    <col min="9" max="14" width="7.33203125" customWidth="1"/>
+    <col min="15" max="15" width="8.21875" customWidth="1"/>
+    <col min="16" max="1023" width="7.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75">
+    <row r="1" spans="1:20" ht="15.75">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -5074,23 +6179,31 @@
       <c r="C1" s="20">
         <v>12</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22" t="s">
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
     </row>
-    <row r="2" spans="1:15" ht="15.75">
+    <row r="2" spans="1:20" ht="15.75">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -5129,11 +6242,17 @@
       <c r="M2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="21" t="s">
+      <c r="N2" s="30" t="s">
         <v>12</v>
       </c>
+      <c r="O2" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" s="32" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75">
+    <row r="3" spans="1:20" ht="15.75">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -5184,8 +6303,16 @@
         <f>8*C1</f>
         <v>96</v>
       </c>
+      <c r="O3" s="31">
+        <f>C1</f>
+        <v>12</v>
+      </c>
+      <c r="P3" s="31">
+        <f>C1</f>
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:20">
       <c r="A4" s="4" t="s">
         <v>22</v>
       </c>
@@ -5228,8 +6355,12 @@
       <c r="N4" s="6">
         <v>371.32100000000003</v>
       </c>
+      <c r="O4" s="6">
+        <v>359.572</v>
+      </c>
+      <c r="P4" s="6"/>
     </row>
-    <row r="5" spans="1:15" ht="15.75">
+    <row r="5" spans="1:20" ht="15.75">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -5282,8 +6413,13 @@
         <f>C4/N4</f>
         <v>184.83326017111878</v>
       </c>
+      <c r="O5" s="16">
+        <f>D4/O4</f>
+        <v>190.87267918525359</v>
+      </c>
+      <c r="P5" s="16"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:20">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -5297,58 +6433,69 @@
         <v>1</v>
       </c>
       <c r="E6" s="16">
-        <f>E5/E3</f>
+        <f t="shared" ref="E6:P6" si="0">E5/E3</f>
         <v>0.25059556201489253</v>
       </c>
       <c r="F6" s="16">
-        <f>F5/F3</f>
+        <f t="shared" si="0"/>
         <v>0.25811342808368859</v>
       </c>
       <c r="G6" s="16">
-        <f>G5/G3</f>
+        <f t="shared" si="0"/>
         <v>15.239874719106114</v>
       </c>
       <c r="H6" s="16">
-        <f>H5/H3</f>
+        <f t="shared" si="0"/>
         <v>16.074684045343826</v>
       </c>
       <c r="I6" s="16">
-        <f>I5/I3</f>
+        <f t="shared" si="0"/>
         <v>44.399838398946301</v>
       </c>
       <c r="J6" s="16">
-        <f>J5/J3</f>
+        <f t="shared" si="0"/>
         <v>25.642006318548709</v>
       </c>
       <c r="K6" s="16">
-        <f>K5/K3</f>
+        <f t="shared" si="0"/>
         <v>16.074684045343826</v>
       </c>
       <c r="L6" s="16">
-        <f>L5/L3</f>
+        <f t="shared" si="0"/>
         <v>7.8322249017212711</v>
       </c>
       <c r="M6" s="16">
-        <f>M5/M3</f>
+        <f t="shared" si="0"/>
         <v>3.8773724959278604</v>
       </c>
       <c r="N6" s="16">
-        <f>N5/N3</f>
+        <f t="shared" si="0"/>
         <v>1.9253464601158206</v>
       </c>
+      <c r="O6" s="16">
+        <f t="shared" si="0"/>
+        <v>15.906056598771132</v>
+      </c>
+      <c r="P6" s="16"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:20">
       <c r="L8" s="9"/>
     </row>
-    <row r="9" spans="1:15">
-      <c r="C9" t="s">
+    <row r="9" spans="1:20">
+      <c r="C9" s="33" t="s">
         <v>20</v>
       </c>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:20">
       <c r="O10" s="9"/>
     </row>
-    <row r="11" spans="1:15" ht="58.15" customHeight="1">
+    <row r="11" spans="1:20" ht="58.15" customHeight="1">
       <c r="C11" s="12" t="s">
         <v>23</v>
       </c>
@@ -5362,7 +6509,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:20">
       <c r="C12" s="10" t="s">
         <v>24</v>
       </c>
@@ -5376,7 +6523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:20">
       <c r="C13" s="10" t="s">
         <v>25</v>
       </c>
@@ -5390,7 +6537,7 @@
         <v>0.25059556201489253</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:20">
       <c r="C14" s="10" t="s">
         <v>26</v>
       </c>
@@ -5405,21 +6552,21 @@
       </c>
       <c r="L14" s="9"/>
     </row>
-    <row r="15" spans="1:15">
-      <c r="C15" s="23" t="s">
+    <row r="15" spans="1:20">
+      <c r="C15" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="23">
         <v>375.29</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E15" s="23">
         <v>182.87849662927337</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15" s="24">
         <v>15.239874719106114</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:20">
       <c r="C16" s="18" t="s">
         <v>35</v>
       </c>
@@ -5433,12 +6580,18 @@
         <v>16.07</v>
       </c>
     </row>
-    <row r="35" spans="3:7">
-      <c r="C35" t="s">
+    <row r="35" spans="3:9">
+      <c r="C35" s="33" t="s">
         <v>21</v>
       </c>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
     </row>
-    <row r="37" spans="3:7" ht="65.45" customHeight="1">
+    <row r="37" spans="3:9" ht="65.45" customHeight="1">
       <c r="C37" s="17" t="s">
         <v>23</v>
       </c>
@@ -5449,7 +6602,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="3:7">
+    <row r="38" spans="3:9">
       <c r="C38" s="18" t="s">
         <v>31</v>
       </c>
@@ -5460,81 +6613,81 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="3:7">
-      <c r="C39" s="26">
+    <row r="39" spans="3:9">
+      <c r="C39" s="25">
         <v>1</v>
       </c>
-      <c r="D39" s="27">
+      <c r="D39" s="26">
         <f>I5</f>
         <v>44.399838398946301</v>
       </c>
-      <c r="E39" s="27">
+      <c r="E39" s="26">
         <f>I6</f>
         <v>44.399838398946301</v>
       </c>
     </row>
-    <row r="40" spans="3:7">
+    <row r="40" spans="3:9">
       <c r="C40" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D40" s="27">
+      <c r="D40" s="26">
         <f>J5</f>
         <v>153.85203791129226</v>
       </c>
-      <c r="E40" s="27">
+      <c r="E40" s="26">
         <f>J6</f>
         <v>25.642006318548709</v>
       </c>
     </row>
-    <row r="41" spans="3:7">
+    <row r="41" spans="3:9">
       <c r="C41" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D41" s="27">
+      <c r="D41" s="26">
         <f>K5</f>
         <v>192.89620854412593</v>
       </c>
-      <c r="E41" s="27">
+      <c r="E41" s="26">
         <f>K6</f>
         <v>16.074684045343826</v>
       </c>
     </row>
-    <row r="42" spans="3:7">
+    <row r="42" spans="3:9">
       <c r="C42" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D42" s="27">
+      <c r="D42" s="26">
         <f>L5</f>
         <v>187.9733976413105</v>
       </c>
-      <c r="E42" s="27">
+      <c r="E42" s="26">
         <f>L6</f>
         <v>7.8322249017212711</v>
       </c>
       <c r="G42" s="9"/>
     </row>
-    <row r="43" spans="3:7">
+    <row r="43" spans="3:9">
       <c r="C43" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D43" s="27">
+      <c r="D43" s="26">
         <f>M5</f>
         <v>186.11387980453731</v>
       </c>
-      <c r="E43" s="27">
+      <c r="E43" s="26">
         <f>M6</f>
         <v>3.8773724959278604</v>
       </c>
     </row>
-    <row r="44" spans="3:7">
+    <row r="44" spans="3:9">
       <c r="C44" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D44" s="27">
+      <c r="D44" s="26">
         <f>N5</f>
         <v>184.83326017111878</v>
       </c>
-      <c r="E44" s="27">
+      <c r="E44" s="26">
         <f>N6</f>
         <v>1.9253464601158206</v>
       </c>
@@ -5542,10 +6695,66 @@
     <row r="60" spans="14:14">
       <c r="N60" s="9"/>
     </row>
+    <row r="65" spans="3:9">
+      <c r="C65" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D65" s="34"/>
+      <c r="E65" s="34"/>
+      <c r="F65" s="34"/>
+      <c r="G65" s="34"/>
+      <c r="H65" s="34"/>
+      <c r="I65" s="34"/>
+    </row>
+    <row r="67" spans="3:9" ht="51">
+      <c r="C67" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E67" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F67" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="68" spans="3:9">
+      <c r="C68" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D68" s="11">
+        <v>22823.119999999999</v>
+      </c>
+      <c r="E68" s="11">
+        <v>3.01</v>
+      </c>
+      <c r="F68" s="19">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="69" spans="3:9">
+      <c r="C69" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D69" s="11">
+        <v>359.572</v>
+      </c>
+      <c r="E69" s="11">
+        <v>190.87</v>
+      </c>
+      <c r="F69" s="16">
+        <v>15.91</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
+    <mergeCell ref="C35:I35"/>
     <mergeCell ref="D1:H1"/>
     <mergeCell ref="I1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="C9:I9"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39370000000000005" bottom="0.39370000000000005" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>